<commit_message>
delete file no use
</commit_message>
<xml_diff>
--- a/dcomtestcasegeneration/Database/Database.xlsx
+++ b/dcomtestcasegeneration/Database/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BOSCH_WORK\DCOM_TestcaseTool\dcomtestcasegeneration\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HuyNA_repo\dcomtestcasegeneration\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A07B351-88DA-4FA4-BF8D-5F8511E1F55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CEE65C-7BD8-4D0B-90EB-24EC499057C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="2280" windowWidth="12555" windowHeight="12915" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common_settings" sheetId="2" r:id="rId1"/>
@@ -658,16 +658,16 @@
     <t>Database Directory</t>
   </si>
   <si>
-    <t>D:\BOSCH_WORK\DCOM_TestcaseTool\dcomtestcasegeneration\Template\Template.xlsx</t>
+    <t>D:\HuyNA_repo\dcomtestcasegeneration\Database\Database.xlsx</t>
   </si>
   <si>
-    <t>D:\BOSCH_WORK\DCOM_TestcaseTool\dcomtestcasegeneration\Template</t>
+    <t>D:\HuyNA_repo\dcomtestcasegeneration\Template</t>
   </si>
   <si>
-    <t>D:\BOSCH_WORK\DCOM_TestcaseTool\dcomtestcasegeneration\Database\Database.xlsx</t>
+    <t>D:\HuyNA_repo\dcomtestcasegeneration\Template\Template.xlsx</t>
   </si>
   <si>
-    <t>D:\BOSCH_WORK\DCOM_TestcaseTool\dcomtestcasegeneration\Database</t>
+    <t>D:\HuyNA_repo\dcomtestcasegeneration\Database</t>
   </si>
 </sst>
 </file>
@@ -10798,21 +10798,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -10854,7 +10854,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -10868,7 +10868,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -10882,7 +10882,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>60</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
@@ -10940,13 +10940,13 @@
         <v>590209</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>92</v>
       </c>
@@ -10956,7 +10956,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>97</v>
       </c>
@@ -10966,7 +10966,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>95</v>
       </c>
@@ -10976,7 +10976,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>107</v>
       </c>
@@ -10986,43 +10986,43 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>182</v>
       </c>
@@ -11032,7 +11032,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>170</v>
       </c>
@@ -11042,7 +11042,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>171</v>
       </c>
@@ -11052,7 +11052,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>172</v>
       </c>
@@ -11062,7 +11062,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>173</v>
       </c>
@@ -11070,7 +11070,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>181</v>
       </c>
@@ -11078,7 +11078,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>177</v>
       </c>
@@ -11086,27 +11086,27 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>178</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B43" s="9"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>194</v>
       </c>
       <c r="B44" s="9"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>179</v>
       </c>
@@ -11114,15 +11114,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>196</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>183</v>
       </c>
@@ -11138,7 +11138,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>41</v>
       </c>
@@ -11146,7 +11146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>19</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>81</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>184</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>23</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>185</v>
       </c>
@@ -11186,7 +11186,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>186</v>
       </c>
@@ -11194,7 +11194,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>187</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>188</v>
       </c>
@@ -11210,7 +11210,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>21</v>
       </c>
@@ -11218,7 +11218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>189</v>
       </c>
@@ -11226,7 +11226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>190</v>
       </c>
@@ -11254,31 +11254,31 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -11312,7 +11312,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
@@ -11458,7 +11458,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -11504,7 +11504,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
@@ -11542,7 +11542,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
@@ -11582,7 +11582,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>15</v>
       </c>
@@ -11624,7 +11624,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
@@ -11668,7 +11668,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
@@ -11714,7 +11714,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
@@ -11762,7 +11762,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>15</v>
       </c>
@@ -11812,7 +11812,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -11864,7 +11864,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -11918,7 +11918,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>14</v>
       </c>
@@ -11974,7 +11974,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -12028,7 +12028,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -12084,7 +12084,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -12112,7 +12112,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -12123,7 +12123,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -12134,7 +12134,7 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
@@ -12144,7 +12144,7 @@
       <c r="H20" s="37"/>
       <c r="I20" s="21"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -12154,7 +12154,7 @@
       <c r="H21" s="37"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -12164,7 +12164,7 @@
       <c r="H22" s="37"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -12174,45 +12174,45 @@
       <c r="H23" s="37"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
       <c r="D27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -12220,7 +12220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -12242,7 +12242,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -12272,7 +12272,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -12313,31 +12313,31 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="42" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
         <v>29</v>
       </c>
@@ -12371,7 +12371,7 @@
       <c r="Y1" s="67"/>
       <c r="Z1" s="67"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
@@ -12447,7 +12447,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -12563,7 +12563,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -12597,7 +12597,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -12633,7 +12633,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -12671,7 +12671,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="70"/>
       <c r="C8" s="21"/>
@@ -12711,7 +12711,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -12753,7 +12753,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -12797,7 +12797,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -12843,7 +12843,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -12891,7 +12891,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -12941,7 +12941,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -12993,7 +12993,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -13047,7 +13047,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="71"/>
@@ -13103,7 +13103,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -13131,7 +13131,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -13158,7 +13158,7 @@
       <c r="Y18" s="37"/>
       <c r="Z18" s="34"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -13185,69 +13185,69 @@
       <c r="Y19" s="37"/>
       <c r="Z19" s="34"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
       <c r="I34" s="72"/>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
       <c r="I37" s="102"/>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
       <c r="I38" s="102"/>
     </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -13255,7 +13255,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -13288,7 +13288,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -13299,7 +13299,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -13307,7 +13307,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="101"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -13348,31 +13348,31 @@
       <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -13406,7 +13406,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -13482,7 +13482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
@@ -13550,7 +13550,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
@@ -13594,7 +13594,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -13628,7 +13628,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -13664,7 +13664,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -13702,7 +13702,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -13742,7 +13742,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -13784,7 +13784,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -13828,7 +13828,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -13874,7 +13874,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -13922,7 +13922,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -13972,7 +13972,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -14024,7 +14024,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -14078,7 +14078,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -14134,7 +14134,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -14162,7 +14162,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -14189,7 +14189,7 @@
       <c r="Y18" s="37"/>
       <c r="Z18" s="34"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -14216,60 +14216,60 @@
       <c r="Y19" s="37"/>
       <c r="Z19" s="34"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -14277,7 +14277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -14288,7 +14288,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -14299,7 +14299,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -14321,7 +14321,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -14329,7 +14329,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -14370,31 +14370,31 @@
       <selection activeCell="N32" sqref="M32:N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -14428,7 +14428,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -14504,7 +14504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
@@ -14574,7 +14574,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -14620,7 +14620,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
@@ -14658,7 +14658,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
@@ -14698,7 +14698,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>12</v>
       </c>
@@ -14740,7 +14740,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
@@ -14784,7 +14784,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -14826,7 +14826,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -14870,7 +14870,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -14916,7 +14916,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -14964,7 +14964,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -15014,7 +15014,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -15066,7 +15066,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -15120,7 +15120,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -15176,7 +15176,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -15204,7 +15204,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -15215,7 +15215,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -15226,60 +15226,60 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -15287,7 +15287,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -15298,7 +15298,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -15309,7 +15309,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -15331,7 +15331,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -15339,7 +15339,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -15377,7 +15377,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15392,34 +15392,34 @@
       <selection activeCell="G8" sqref="G8:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="21" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="21" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -15453,7 +15453,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -15529,7 +15529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
         <v>12</v>
       </c>
@@ -15603,7 +15603,7 @@
       </c>
       <c r="Z3" s="56"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>13</v>
       </c>
@@ -15677,7 +15677,7 @@
       </c>
       <c r="Z4" s="59"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>14</v>
       </c>
@@ -15751,7 +15751,7 @@
       </c>
       <c r="Z5" s="59"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="53"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -15817,7 +15817,7 @@
       </c>
       <c r="Z6" s="59"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -15883,7 +15883,7 @@
       </c>
       <c r="Z7" s="59"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="53"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -15941,7 +15941,7 @@
       </c>
       <c r="Z8" s="59"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -15999,7 +15999,7 @@
       </c>
       <c r="Z9" s="59"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="53"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -16057,7 +16057,7 @@
       </c>
       <c r="Z10" s="59"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="53"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -16115,7 +16115,7 @@
       </c>
       <c r="Z11" s="59"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -16173,7 +16173,7 @@
       </c>
       <c r="Z12" s="59"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="53"/>
       <c r="B13" s="53"/>
       <c r="C13" s="25"/>
@@ -16231,7 +16231,7 @@
       </c>
       <c r="Z13" s="59"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="53"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -16289,7 +16289,7 @@
       </c>
       <c r="Z14" s="59"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="53"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -16347,7 +16347,7 @@
       </c>
       <c r="Z15" s="59"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="53"/>
       <c r="B16" s="25"/>
       <c r="C16" s="61"/>
@@ -16405,7 +16405,7 @@
       </c>
       <c r="Z16" s="59"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
       <c r="B17" s="61"/>
       <c r="C17" s="63"/>
@@ -16432,11 +16432,11 @@
       <c r="Y17" s="64"/>
       <c r="Z17" s="59"/>
     </row>
-    <row r="38" spans="5:5" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:5" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -16455,7 +16455,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -16466,7 +16466,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -16477,7 +16477,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -16488,7 +16488,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -16496,7 +16496,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -16538,30 +16538,30 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
     <col min="4" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -16595,7 +16595,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -16671,7 +16671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
@@ -16745,7 +16745,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -16813,7 +16813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -16873,7 +16873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -16933,7 +16933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -16993,7 +16993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -17053,7 +17053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -17113,7 +17113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -17173,7 +17173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -17233,7 +17233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -17293,7 +17293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -17353,7 +17353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -17413,7 +17413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -17473,7 +17473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -17533,7 +17533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -17561,12 +17561,12 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="I25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -17574,7 +17574,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -17585,7 +17585,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -17596,7 +17596,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -17607,7 +17607,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -17618,7 +17618,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -17626,7 +17626,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -17667,31 +17667,31 @@
       <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -17725,7 +17725,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -17801,7 +17801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>91</v>
       </c>
@@ -17875,7 +17875,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -17917,7 +17917,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -17951,7 +17951,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -17987,7 +17987,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -18025,7 +18025,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -18065,7 +18065,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -18107,7 +18107,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -18151,7 +18151,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -18197,7 +18197,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -18245,7 +18245,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -18295,7 +18295,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -18347,7 +18347,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -18401,7 +18401,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -18457,7 +18457,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -18485,10 +18485,10 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -18496,7 +18496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -18507,7 +18507,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -18518,7 +18518,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -18529,7 +18529,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -18540,7 +18540,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -18548,7 +18548,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -18589,31 +18589,31 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -18647,7 +18647,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -18723,7 +18723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -18839,7 +18839,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>35</v>
       </c>
@@ -18879,7 +18879,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>35</v>
       </c>
@@ -18921,7 +18921,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>35</v>
       </c>
@@ -18965,7 +18965,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>71</v>
       </c>
@@ -19011,7 +19011,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>71</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>71</v>
       </c>
@@ -19109,7 +19109,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -19161,7 +19161,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
@@ -19215,7 +19215,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>36</v>
       </c>
@@ -19271,7 +19271,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>36</v>
       </c>
@@ -19329,7 +19329,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>72</v>
       </c>
@@ -19389,7 +19389,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>72</v>
       </c>
@@ -19451,7 +19451,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
         <v>72</v>
       </c>
@@ -19485,7 +19485,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>72</v>
       </c>
@@ -19502,7 +19502,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37" t="s">
         <v>73</v>
       </c>
@@ -19515,60 +19515,60 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -19576,7 +19576,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -19587,7 +19587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -19598,7 +19598,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -19609,7 +19609,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -19620,7 +19620,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -19628,7 +19628,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -19669,31 +19669,31 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" style="78" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="78" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="78" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="78" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="78" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="78" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="78" customWidth="1"/>
     <col min="5" max="5" width="9" style="78" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="78" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="78" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="78" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="78" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="78" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="78" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="78" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="78" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="78" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="78" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="78" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="78" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="78" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="78" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="78"/>
+    <col min="6" max="6" width="17.7109375" style="78" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="78" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="78" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="78" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="78" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="78" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="78" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="78" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="78" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="78" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="78" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="78" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="78" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="78" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -19727,7 +19727,7 @@
       <c r="Y1" s="76"/>
       <c r="Z1" s="77"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="79" t="s">
         <v>109</v>
       </c>
@@ -19803,7 +19803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
         <v>152</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="82" t="s">
         <v>110</v>
       </c>
@@ -19923,7 +19923,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="82" t="s">
         <v>111</v>
       </c>
@@ -19963,7 +19963,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="82" t="s">
         <v>111</v>
       </c>
@@ -20005,7 +20005,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="82" t="s">
         <v>111</v>
       </c>
@@ -20049,7 +20049,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="82" t="s">
         <v>111</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="82" t="s">
         <v>111</v>
       </c>
@@ -20143,7 +20143,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
         <v>111</v>
       </c>
@@ -20193,7 +20193,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="82" t="s">
         <v>111</v>
       </c>
@@ -20245,7 +20245,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="82" t="s">
         <v>111</v>
       </c>
@@ -20299,7 +20299,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="82" t="s">
         <v>111</v>
       </c>
@@ -20355,7 +20355,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="82" t="s">
         <v>111</v>
       </c>
@@ -20413,7 +20413,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
         <v>111</v>
       </c>
@@ -20473,7 +20473,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="82" t="s">
         <v>111</v>
       </c>
@@ -20535,7 +20535,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="82" t="s">
         <v>111</v>
       </c>
@@ -20569,7 +20569,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="82" t="s">
         <v>111</v>
       </c>
@@ -20586,7 +20586,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="82" t="s">
         <v>111</v>
       </c>
@@ -20603,7 +20603,7 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="82" t="s">
         <v>112</v>
       </c>
@@ -20615,7 +20615,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="82" t="s">
         <v>113</v>
       </c>
@@ -20627,7 +20627,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="82" t="s">
         <v>114</v>
       </c>
@@ -20639,7 +20639,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="82" t="s">
         <v>115</v>
       </c>
@@ -20651,7 +20651,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="82" t="s">
         <v>116</v>
       </c>
@@ -20663,7 +20663,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="82" t="s">
         <v>117</v>
       </c>
@@ -20675,7 +20675,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="82" t="s">
         <v>118</v>
       </c>
@@ -20687,7 +20687,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="84" t="s">
         <v>119</v>
       </c>
@@ -20699,7 +20699,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="82" t="s">
         <v>120</v>
       </c>
@@ -20711,7 +20711,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="82" t="s">
         <v>121</v>
       </c>
@@ -20723,7 +20723,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="82" t="s">
         <v>122</v>
       </c>
@@ -20735,7 +20735,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="85" t="s">
         <v>123</v>
       </c>
@@ -20747,7 +20747,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="85" t="s">
         <v>124</v>
       </c>
@@ -20759,7 +20759,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="85" t="s">
         <v>125</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="96" t="s">
         <v>126</v>
       </c>
@@ -20783,7 +20783,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
         <v>127</v>
       </c>
@@ -20795,7 +20795,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="96" t="s">
         <v>128</v>
       </c>
@@ -20807,7 +20807,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
         <v>129</v>
       </c>
@@ -20819,7 +20819,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="96" t="s">
         <v>130</v>
       </c>
@@ -20831,100 +20831,100 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="38"/>
       <c r="B39" s="38"/>
       <c r="C39" s="37"/>
       <c r="D39" s="52"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
       <c r="C40" s="37"/>
       <c r="D40" s="40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="38"/>
       <c r="B41" s="38"/>
       <c r="C41" s="37"/>
       <c r="D41" s="40"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="38"/>
       <c r="B42" s="38"/>
       <c r="C42" s="37"/>
       <c r="D42" s="40"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="38"/>
       <c r="B43" s="38"/>
       <c r="C43" s="37"/>
       <c r="D43" s="40"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="38"/>
       <c r="B44" s="38"/>
       <c r="C44" s="37"/>
       <c r="D44" s="40"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
       <c r="C45" s="37"/>
       <c r="D45" s="40"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
       <c r="C46" s="37"/>
       <c r="D46" s="40"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
       <c r="C47" s="37"/>
       <c r="D47" s="40"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
       <c r="C48" s="37"/>
       <c r="D48" s="40"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
       <c r="C49" s="37"/>
       <c r="D49" s="40"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
       <c r="C50" s="37"/>
       <c r="D50" s="40"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="38"/>
       <c r="B51" s="38"/>
       <c r="C51" s="37"/>
       <c r="D51" s="40"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="37"/>
       <c r="D52" s="40"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="37"/>
       <c r="B53" s="37"/>
       <c r="C53" s="37"/>
       <c r="D53" s="86"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E64" s="95"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="87" t="s">
         <v>65</v>
       </c>
@@ -20932,7 +20932,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="89" t="s">
         <v>86</v>
       </c>
@@ -20943,7 +20943,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="90" t="s">
         <v>87</v>
       </c>
@@ -20954,7 +20954,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="90" t="s">
         <v>88</v>
       </c>
@@ -20965,7 +20965,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="92" t="s">
         <v>89</v>
       </c>
@@ -20976,7 +20976,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="94" t="s">
         <v>66</v>
       </c>
@@ -20984,7 +20984,7 @@
       <c r="C110" s="94"/>
       <c r="D110" s="94"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="78" t="s">
         <v>7</v>
       </c>
@@ -21025,31 +21025,31 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -21083,7 +21083,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -21159,7 +21159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="20" t="s">
         <v>100</v>
@@ -21229,7 +21229,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="20" t="s">
         <v>76</v>
@@ -21275,7 +21275,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="20" t="s">
         <v>100</v>
@@ -21313,7 +21313,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>102</v>
@@ -21353,7 +21353,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
         <v>103</v>
@@ -21395,7 +21395,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="20" t="s">
         <v>104</v>
@@ -21439,7 +21439,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="20" t="s">
         <v>104</v>
@@ -21485,7 +21485,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="20" t="s">
         <v>105</v>
@@ -21533,7 +21533,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -21579,7 +21579,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -21627,7 +21627,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -21677,7 +21677,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -21729,7 +21729,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -21783,7 +21783,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -21839,7 +21839,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -21867,7 +21867,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -21878,7 +21878,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -21889,70 +21889,70 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
       <c r="D26" s="42"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
       <c r="D27" s="42"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
       <c r="D29" s="42"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -21960,7 +21960,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -21971,7 +21971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -21982,7 +21982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -21993,7 +21993,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -22004,7 +22004,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -22012,7 +22012,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -22053,31 +22053,31 @@
       <selection activeCell="A100" sqref="A100:D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -22111,7 +22111,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -22187,7 +22187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
@@ -22257,7 +22257,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
@@ -22303,7 +22303,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -22337,7 +22337,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -22373,7 +22373,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -22411,7 +22411,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -22451,7 +22451,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -22493,7 +22493,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -22537,7 +22537,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -22583,7 +22583,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -22631,7 +22631,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -22681,7 +22681,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -22733,7 +22733,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -22787,7 +22787,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -22843,7 +22843,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -22871,7 +22871,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -22882,7 +22882,7 @@
       <c r="H18" s="37"/>
       <c r="I18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -22893,60 +22893,60 @@
       <c r="H19" s="37"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -22954,7 +22954,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -22965,7 +22965,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -22976,7 +22976,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -22987,7 +22987,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -22998,7 +22998,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -23006,7 +23006,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>
@@ -23047,31 +23047,31 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="7.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="5.109375" style="2" customWidth="1"/>
-    <col min="20" max="24" width="4.88671875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="2" customWidth="1"/>
+    <col min="20" max="24" width="4.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
         <v>29</v>
       </c>
@@ -23105,7 +23105,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -23181,7 +23181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -23247,7 +23247,7 @@
       </c>
       <c r="Z3" s="29"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -23289,7 +23289,7 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="34"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -23323,7 +23323,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="34"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -23359,7 +23359,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="34"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -23397,7 +23397,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="34"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -23437,7 +23437,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="34"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -23479,7 +23479,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -23523,7 +23523,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="34"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -23569,7 +23569,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="34"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -23617,7 +23617,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="34"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
@@ -23667,7 +23667,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="34"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -23719,7 +23719,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="34"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -23773,7 +23773,7 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="21"/>
       <c r="C16" s="37"/>
@@ -23829,7 +23829,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="34"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="39"/>
@@ -23857,7 +23857,7 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="34"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -23884,7 +23884,7 @@
       <c r="Y18" s="37"/>
       <c r="Z18" s="34"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -23911,60 +23911,60 @@
       <c r="Y19" s="37"/>
       <c r="Z19" s="34"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="51"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
         <v>65</v>
       </c>
@@ -23972,7 +23972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="45" t="s">
         <v>86</v>
       </c>
@@ -23983,7 +23983,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
         <v>87</v>
       </c>
@@ -23994,7 +23994,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="46" t="s">
         <v>88</v>
       </c>
@@ -24005,7 +24005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="48" t="s">
         <v>89</v>
       </c>
@@ -24016,7 +24016,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="50" t="s">
         <v>66</v>
       </c>
@@ -24024,7 +24024,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>